<commit_message>
Added power draw to xls file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\achin\Documents\Athena Project\motor testing\final data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A3E0ADC5-B915-438E-BF42-44905F453FFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343BEC85-5AEC-4865-B8E7-321E84C4D912}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t/>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Instantaneous Kt (Nm/A)</t>
+  </si>
+  <si>
+    <t>Power draw (W)</t>
   </si>
 </sst>
 </file>
@@ -1798,16 +1801,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>85844</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>111675</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>167788</xdr:rowOff>
+      <xdr:rowOff>64466</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>551818</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>25709</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>116116</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2158,10 +2161,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet 1"/>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="59" workbookViewId="0">
+      <selection activeCell="AC16" sqref="AC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2175,7 +2178,7 @@
     <col min="7" max="7" width="17.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2194,8 +2197,11 @@
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0.117624416947364</v>
       </c>
@@ -2217,8 +2223,12 @@
         <f>E2/D2</f>
         <v>2.1560149378974946E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <f>B2*D2</f>
+        <v>1.3882236779419659</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>-0.55252170562744096</v>
       </c>
@@ -2240,8 +2250,12 @@
         <f t="shared" ref="F3:F40" si="2">E3/D3</f>
         <v>9.1797298610020433E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <f t="shared" ref="G3:G40" si="3">B3*D3</f>
+        <v>6.5209565686700186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>-0.1273894906044</v>
       </c>
@@ -2263,8 +2277,12 @@
         <f t="shared" si="2"/>
         <v>3.9814901338688723E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <f t="shared" si="3"/>
+        <v>1.4995727527714691</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>-0.52168047428131104</v>
       </c>
@@ -2286,8 +2304,12 @@
         <f t="shared" si="2"/>
         <v>0.10208547688768245</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>6.1569630312504646</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>-1.4956291913986199</v>
       </c>
@@ -2309,8 +2331,12 @@
         <f t="shared" si="2"/>
         <v>0.35607756458803991</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>17.697463847499147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>-6.2698845863342196</v>
       </c>
@@ -2332,8 +2358,12 @@
         <f t="shared" si="2"/>
         <v>0.15976689621741033</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>73.134472297403377</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>-11.804434776306101</v>
       </c>
@@ -2344,7 +2374,7 @@
         <v>11.5</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" ref="D8:D40" si="3">ABS(A8)</f>
+        <f t="shared" ref="D8:D40" si="4">ABS(A8)</f>
         <v>11.804434776306101</v>
       </c>
       <c r="E8" s="1">
@@ -2355,8 +2385,12 @@
         <f t="shared" si="2"/>
         <v>0.12352984514996886</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>126.669133586507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>-18.058506011962798</v>
       </c>
@@ -2367,7 +2401,7 @@
         <v>15.14</v>
       </c>
       <c r="D9" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>18.058506011962798</v>
       </c>
       <c r="E9" s="1">
@@ -2378,8 +2412,12 @@
         <f t="shared" si="2"/>
         <v>0.10630735448039093</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>191.29143666358971</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>-23.823959350585898</v>
       </c>
@@ -2390,7 +2428,7 @@
         <v>19.579999999999998</v>
       </c>
       <c r="D10" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.823959350585898</v>
       </c>
       <c r="E10" s="1">
@@ -2401,8 +2439,12 @@
         <f t="shared" si="2"/>
         <v>0.10421206498318435</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>248.35255725351323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>-28.792921066284102</v>
       </c>
@@ -2413,7 +2455,7 @@
         <v>20.62</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>28.792921066284102</v>
       </c>
       <c r="E11" s="1">
@@ -2424,8 +2466,12 @@
         <f t="shared" si="2"/>
         <v>9.0807597950235741E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>300.15143462853297</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>-33.160091400146399</v>
       </c>
@@ -2436,7 +2482,7 @@
         <v>26</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33.160091400146399</v>
       </c>
       <c r="E12" s="1">
@@ -2447,8 +2493,12 @@
         <f t="shared" si="2"/>
         <v>9.94207151065164E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>341.10855293195323</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>-37.962413787841797</v>
       </c>
@@ -2459,7 +2509,7 @@
         <v>28.46</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37.962413787841797</v>
       </c>
       <c r="E13" s="1">
@@ -2470,8 +2520,12 @@
         <f t="shared" si="2"/>
         <v>9.5060551738566368E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>384.69755445113714</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>-39.935707092285099</v>
       </c>
@@ -2482,7 +2536,7 @@
         <v>28.38</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.935707092285099</v>
       </c>
       <c r="E14" s="1">
@@ -2493,8 +2547,12 @@
         <f t="shared" si="2"/>
         <v>9.010943493962037E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>402.86022784619541</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>-39.970939636230398</v>
       </c>
@@ -2505,7 +2563,7 @@
         <v>27.8</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.970939636230398</v>
       </c>
       <c r="E15" s="1">
@@ -2516,8 +2574,12 @@
         <f t="shared" si="2"/>
         <v>8.8190070888522196E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>401.99193944403964</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>-39.939208984375</v>
       </c>
@@ -2528,7 +2590,7 @@
         <v>28.62</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.939208984375</v>
       </c>
       <c r="E16" s="1">
@@ -2539,8 +2601,12 @@
         <f t="shared" si="2"/>
         <v>9.0863492099198612E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>394.33630862832069</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>-39.779346466064403</v>
       </c>
@@ -2551,7 +2617,7 @@
         <v>28.04</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.779346466064403</v>
       </c>
       <c r="E17" s="1">
@@ -2562,8 +2628,12 @@
         <f t="shared" si="2"/>
         <v>8.93798494913223E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>391.54008110735515</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>-39.649360656738203</v>
       </c>
@@ -2574,7 +2644,7 @@
         <v>28.52</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.649360656738203</v>
       </c>
       <c r="E18" s="1">
@@ -2585,8 +2655,12 @@
         <f t="shared" si="2"/>
         <v>9.1207927192274219E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>389.04675985612892</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>-39.825847625732401</v>
       </c>
@@ -2597,7 +2671,7 @@
         <v>28.6</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.825847625732401</v>
       </c>
       <c r="E19" s="1">
@@ -2608,8 +2682,12 @@
         <f t="shared" si="2"/>
         <v>9.1058451136564064E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>384.07246266212292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>-39.972015380859297</v>
       </c>
@@ -2620,7 +2698,7 @@
         <v>28.48</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.972015380859297</v>
       </c>
       <c r="E20" s="1">
@@ -2631,8 +2709,12 @@
         <f t="shared" si="2"/>
         <v>9.0344806625118609E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>384.87020640211904</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>-39.795619964599602</v>
       </c>
@@ -2643,7 +2725,7 @@
         <v>28.18</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.795619964599602</v>
       </c>
       <c r="E21" s="1">
@@ -2654,8 +2736,12 @@
         <f t="shared" si="2"/>
         <v>8.9789378911010298E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>384.39012170485842</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>-39.665859222412102</v>
       </c>
@@ -2666,7 +2752,7 @@
         <v>27.98</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.665859222412102</v>
       </c>
       <c r="E22" s="1">
@@ -2677,8 +2763,12 @@
         <f t="shared" si="2"/>
         <v>8.9443770273741535E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>393.45899800801237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>-39.847862243652301</v>
       </c>
@@ -2689,7 +2779,7 @@
         <v>28.64</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.847862243652301</v>
       </c>
       <c r="E23" s="1">
@@ -2700,8 +2790,12 @@
         <f t="shared" si="2"/>
         <v>9.1135428490357731E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>390.38452541828116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>-39.983993530273402</v>
       </c>
@@ -2712,7 +2806,7 @@
         <v>29.32</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.983993530273402</v>
       </c>
       <c r="E24" s="1">
@@ -2723,8 +2817,12 @@
         <f t="shared" si="2"/>
         <v>9.2981607682212392E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>388.65788828395273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>-39.8133735656738</v>
       </c>
@@ -2735,7 +2833,7 @@
         <v>28.5</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.8133735656738</v>
       </c>
       <c r="E25" s="1">
@@ -2746,8 +2844,12 @@
         <f t="shared" si="2"/>
         <v>9.0768495014342046E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>385.78052416840308</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>-39.649158477783203</v>
       </c>
@@ -2758,7 +2860,7 @@
         <v>28.58</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.649158477783203</v>
       </c>
       <c r="E26" s="1">
@@ -2769,8 +2871,12 @@
         <f t="shared" si="2"/>
         <v>9.1400275292869607E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>373.871422544729</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>-39.800216674804602</v>
       </c>
@@ -2781,7 +2887,7 @@
         <v>28.62</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.800216674804602</v>
       </c>
       <c r="E27" s="1">
@@ -2792,8 +2898,12 @@
         <f t="shared" si="2"/>
         <v>9.1180810136074888E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>390.52698662552461</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>-39.643863677978501</v>
       </c>
@@ -2804,7 +2914,7 @@
         <v>28.8</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.643863677978501</v>
       </c>
       <c r="E28" s="1">
@@ -2815,8 +2925,12 @@
         <f t="shared" si="2"/>
         <v>9.2116147650576644E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>390.81339688772613</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>-39.796939849853501</v>
       </c>
@@ -2827,7 +2941,7 @@
         <v>28.66</v>
       </c>
       <c r="D29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.796939849853501</v>
       </c>
       <c r="E29" s="1">
@@ -2838,8 +2952,12 @@
         <f t="shared" si="2"/>
         <v>9.131576482289197E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>390.4948338213249</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>-39.661823272705</v>
       </c>
@@ -2850,7 +2968,7 @@
         <v>27.66</v>
       </c>
       <c r="D30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.661823272705</v>
       </c>
       <c r="E30" s="1">
@@ -2861,8 +2979,12 @@
         <f t="shared" si="2"/>
         <v>8.8429822700906741E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>389.77620358469278</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>-39.821090698242102</v>
       </c>
@@ -2873,7 +2995,7 @@
         <v>28.36</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.821090698242102</v>
       </c>
       <c r="E31" s="1">
@@ -2884,8 +3006,12 @@
         <f t="shared" si="2"/>
         <v>9.030511060709713E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>390.73180635146741</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>-39.987880706787102</v>
       </c>
@@ -2896,7 +3022,7 @@
         <v>29.72</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.987880706787102</v>
       </c>
       <c r="E32" s="1">
@@ -2907,8 +3033,12 @@
         <f t="shared" si="2"/>
         <v>9.424095334365587E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>389.91993417055704</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>-39.844692230224602</v>
       </c>
@@ -2919,7 +3049,7 @@
         <v>29.04</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.844692230224602</v>
       </c>
       <c r="E33" s="1">
@@ -2930,8 +3060,12 @@
         <f t="shared" si="2"/>
         <v>9.2415621602085662E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <f t="shared" si="3"/>
+        <v>387.30383271491149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>-39.683094024658203</v>
       </c>
@@ -2942,7 +3076,7 @@
         <v>29.46</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.683094024658203</v>
       </c>
       <c r="E34" s="1">
@@ -2953,8 +3087,12 @@
         <f t="shared" si="2"/>
         <v>9.4133990602618456E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <f t="shared" si="3"/>
+        <v>391.20013379035288</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>-39.862442016601499</v>
       </c>
@@ -2965,7 +3103,7 @@
         <v>30.62</v>
       </c>
       <c r="D35" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.862442016601499</v>
       </c>
       <c r="E35" s="1">
@@ -2976,8 +3114,12 @@
         <f t="shared" si="2"/>
         <v>9.7400354910093273E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <f t="shared" si="3"/>
+        <v>386.86617521925581</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>-39.679435729980398</v>
       </c>
@@ -2988,7 +3130,7 @@
         <v>30.66</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.679435729980398</v>
       </c>
       <c r="E36" s="1">
@@ -2999,8 +3141,12 @@
         <f t="shared" si="2"/>
         <v>9.7977401353583224E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>382.66049579344622</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>-39.905971527099602</v>
       </c>
@@ -3011,7 +3157,7 @@
         <v>30.26</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.905971527099602</v>
       </c>
       <c r="E37" s="1">
@@ -3022,8 +3168,12 @@
         <f t="shared" si="2"/>
         <v>9.6150221462328447E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <f t="shared" si="3"/>
+        <v>390.95381480455393</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>-39.719596862792898</v>
       </c>
@@ -3034,7 +3184,7 @@
         <v>29.32</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.719596862792898</v>
       </c>
       <c r="E38" s="1">
@@ -3045,8 +3195,12 @@
         <f t="shared" si="2"/>
         <v>9.3600547176817012E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <f t="shared" si="3"/>
+        <v>383.04780167899958</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>-39.849834442138601</v>
       </c>
@@ -3057,7 +3211,7 @@
         <v>27.72</v>
       </c>
       <c r="D39" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.849834442138601</v>
       </c>
       <c r="E39" s="1">
@@ -3068,8 +3222,12 @@
         <f t="shared" si="2"/>
         <v>8.8203528300815889E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39">
+        <f t="shared" si="3"/>
+        <v>383.69378828419855</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>-39.819545745849602</v>
       </c>
@@ -3080,7 +3238,7 @@
         <v>23.44</v>
       </c>
       <c r="D40" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>39.819545745849602</v>
       </c>
       <c r="E40" s="1">
@@ -3091,8 +3249,12 @@
         <f t="shared" si="2"/>
         <v>7.4641534561197057E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <f t="shared" si="3"/>
+        <v>382.79261906452996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>